<commit_message>
working on lysimeter water vwc things
</commit_message>
<xml_diff>
--- a/Lysimeter/porewater_sites_complete_key.xlsx
+++ b/Lysimeter/porewater_sites_complete_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/GitHub/TEMPEST/Lysimeter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFE0564-2E23-2B4B-B7ED-E210EBD0181F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28606D0D-2421-6446-B660-2540A9DD683E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2800" windowWidth="27640" windowHeight="16940" xr2:uid="{9FDA7C09-3B14-914C-914F-EB14D3DDCCA0}"/>
+    <workbookView xWindow="4240" yWindow="-19020" windowWidth="27640" windowHeight="16940" xr2:uid="{9FDA7C09-3B14-914C-914F-EB14D3DDCCA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Grid</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>B4</t>
   </si>
   <si>
@@ -77,10 +74,13 @@
     <t>I5</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>S</t>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Freshwater</t>
+  </si>
+  <si>
+    <t>Seawater</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A22" sqref="A22:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,82 +456,82 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -539,7 +539,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -555,7 +555,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -571,7 +571,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -579,7 +579,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -587,7 +587,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -603,7 +603,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -611,7 +611,7 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -619,7 +619,7 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -627,7 +627,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -635,7 +635,7 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -643,7 +643,7 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -651,7 +651,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -659,7 +659,7 @@
         <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -667,7 +667,7 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -675,7 +675,7 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -683,7 +683,7 @@
         <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -691,7 +691,7 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>